<commit_message>
Utilisation des transition système pour l'identification des marquages les plus proches Cas des actions refusées par le jeu : utilisation de RdpW1 au lieu de RdpF
</commit_message>
<xml_diff>
--- a/docs/MatriceLabellisationV10.xlsx
+++ b/docs/MatriceLabellisationV10.xlsx
@@ -21,31 +21,7 @@
     <author>Mathieu MURATET</author>
   </authors>
   <commentList>
-    <comment ref="G53" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Mathieu MURATET:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-L'action est refusée par le jeu on ne l'exécute donc pas dans le Rdp Filtré</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B82" authorId="0">
+    <comment ref="B77" authorId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A88" authorId="0">
+    <comment ref="A83" authorId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B88" authorId="0">
+    <comment ref="B83" authorId="0">
       <text>
         <r>
           <rPr>
@@ -117,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A94" authorId="0">
+    <comment ref="A89" authorId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B94" authorId="0">
+    <comment ref="B89" authorId="0">
       <text>
         <r>
           <rPr>
@@ -165,7 +141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C94" authorId="0">
+    <comment ref="C89" authorId="0">
       <text>
         <r>
           <rPr>
@@ -194,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="132">
   <si>
     <t>C =&gt; Complet</t>
   </si>
@@ -232,25 +208,16 @@
     <t>t == action système</t>
   </si>
   <si>
-    <t>t ϵ RdpF</t>
-  </si>
-  <si>
     <t>Label</t>
   </si>
   <si>
     <t>Précision</t>
   </si>
   <si>
-    <t>NON</t>
-  </si>
-  <si>
     <t>Rattrapage</t>
   </si>
   <si>
     <t>OUI</t>
-  </si>
-  <si>
-    <t>Si t ϵ RdpF &amp;&amp; sens(t, MF) =&gt; Déclancher t ?</t>
   </si>
   <si>
     <t>Erronée</t>
@@ -271,12 +238,6 @@
       </rPr>
       <t>Ø</t>
     </r>
-  </si>
-  <si>
-    <t>amont_t(t, GF, MF)</t>
-  </si>
-  <si>
-    <t>v(t, GF, MF, lSys)</t>
   </si>
   <si>
     <t>Cette transition a pû être faites et pourra être faite</t>
@@ -615,21 +576,6 @@
     <t>Initialiser RdpW1 à RdpW2</t>
   </si>
   <si>
-    <t>Sinon</t>
-  </si>
-  <si>
-    <t>Si RdpW1 == RdpF Alors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Propager M'C dans MF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Si t ϵ RdpF &amp;&amp; sens(t, MF) Alors Déclancher t dans RdpF FinSi</t>
-  </si>
-  <si>
-    <t>FinSi</t>
-  </si>
-  <si>
     <t>Progression dans un puits, on essaye donc d'évaluer la tendance</t>
   </si>
   <si>
@@ -740,6 +686,15 @@
   </si>
   <si>
     <t>Labelliser action courante</t>
+  </si>
+  <si>
+    <t>Si t ϵ RdpW1 &amp;&amp; sens(t, MW1) =&gt; Déclancher t ?</t>
+  </si>
+  <si>
+    <t>amont_t(t, GW1, MC)</t>
+  </si>
+  <si>
+    <t>v(t, GW1, MC, lSys)</t>
   </si>
 </sst>
 </file>
@@ -872,7 +827,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -928,14 +883,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1030,7 +982,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>112</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1078,7 +1030,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>112</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1126,7 +1078,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>112</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1174,7 +1126,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>112</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1222,7 +1174,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>112</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1270,7 +1222,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>112</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4331,27 +4283,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
@@ -4391,12 +4343,12 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
@@ -4409,7 +4361,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -4422,7 +4374,7 @@
     </row>
     <row r="21" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
@@ -4430,12 +4382,12 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
@@ -4455,37 +4407,37 @@
     </row>
     <row r="30" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -4496,10 +4448,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A32:K120"/>
+  <dimension ref="A32:K115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4516,23 +4468,23 @@
   </cols>
   <sheetData>
     <row r="32" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A32" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
+      <c r="A32" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B34" s="3"/>
     </row>
@@ -4541,46 +4493,46 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B36" s="3"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B42" s="3"/>
       <c r="H42" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -4589,7 +4541,7 @@
       </c>
       <c r="B43" s="3"/>
       <c r="H43" s="17" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -4598,7 +4550,7 @@
       </c>
       <c r="B44" s="3"/>
       <c r="H44" s="17" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -4607,7 +4559,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B46" s="3"/>
       <c r="H46" s="17"/>
@@ -4618,13 +4570,13 @@
       </c>
       <c r="B47" s="3"/>
       <c r="G47" s="4" t="s">
-        <v>18</v>
+        <v>129</v>
       </c>
       <c r="H47" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I47" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="I47" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -4633,7 +4585,7 @@
       </c>
       <c r="B48" s="3"/>
       <c r="H48" s="5" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -4642,13 +4594,13 @@
       </c>
       <c r="B49" s="3"/>
       <c r="G49" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -4657,32 +4609,30 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B51" s="3"/>
       <c r="H51" s="17"/>
     </row>
-    <row r="52" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B52" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G52" s="4"/>
+      <c r="H52" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H52" s="6" t="s">
+      <c r="I52" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="I52" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -4698,14 +4648,12 @@
       <c r="D53" s="3">
         <v>1</v>
       </c>
-      <c r="G53" s="28" t="s">
-        <v>15</v>
-      </c>
+      <c r="G53" s="1"/>
       <c r="H53" s="18" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -4721,9 +4669,9 @@
       <c r="D54" s="3">
         <v>0</v>
       </c>
-      <c r="G54" s="28"/>
+      <c r="G54" s="1"/>
       <c r="H54" s="18" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I54" s="3"/>
     </row>
@@ -4740,9 +4688,9 @@
       <c r="D55" s="3">
         <v>1</v>
       </c>
-      <c r="G55" s="28"/>
+      <c r="G55" s="1"/>
       <c r="H55" s="18" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I55" s="3"/>
     </row>
@@ -4759,12 +4707,12 @@
       <c r="D56" s="3">
         <v>0</v>
       </c>
-      <c r="G56" s="28"/>
+      <c r="G56" s="1"/>
       <c r="H56" s="18" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -4776,9 +4724,9 @@
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
-      <c r="G57" s="28"/>
+      <c r="G57" s="1"/>
       <c r="H57" s="19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I57" s="3"/>
     </row>
@@ -4790,8 +4738,8 @@
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="G58" s="26"/>
-      <c r="H58" s="29" t="s">
-        <v>83</v>
+      <c r="H58" s="27" t="s">
+        <v>78</v>
       </c>
       <c r="I58" s="3"/>
     </row>
@@ -4801,7 +4749,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -4814,7 +4762,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -4828,7 +4776,7 @@
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -4840,27 +4788,27 @@
     </row>
     <row r="63" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
       <c r="H63" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I63" s="12" t="s">
         <v>13</v>
-      </c>
-      <c r="I63" s="12" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.25">
@@ -4874,10 +4822,10 @@
       <c r="F64" s="23"/>
       <c r="G64" s="23"/>
       <c r="H64" s="13" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I64" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -4894,7 +4842,7 @@
         <v>1</v>
       </c>
       <c r="H65" s="17" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -4914,7 +4862,7 @@
         <v>1</v>
       </c>
       <c r="H66" s="17" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -4934,10 +4882,10 @@
         <v>0</v>
       </c>
       <c r="H67" s="17" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="I67" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -4951,10 +4899,10 @@
         <v>0</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -4968,10 +4916,10 @@
         <v>1</v>
       </c>
       <c r="H69" s="17" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="I69" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -4985,15 +4933,15 @@
         <v>0</v>
       </c>
       <c r="H70" s="17" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="I70" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B71" s="10"/>
       <c r="H71" s="17"/>
@@ -5001,106 +4949,115 @@
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H72" s="17"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H73" s="17"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="H74" s="17"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="2"/>
-      <c r="B75" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H75" s="17"/>
-    </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="2"/>
-      <c r="B76" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H76" s="17"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="2"/>
-      <c r="B77" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C77" s="2"/>
-      <c r="H77" s="17"/>
+      <c r="A76" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C77" s="11"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I77" s="12" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="2"/>
-      <c r="B78" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C78" s="2"/>
-      <c r="H78" s="17"/>
+      <c r="A78">
+        <v>1</v>
+      </c>
+      <c r="H78" t="s">
+        <v>33</v>
+      </c>
+      <c r="I78" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="2"/>
-      <c r="B79" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H79" s="17"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C82" s="11"/>
-      <c r="F82" s="4"/>
-      <c r="G82" s="4"/>
-      <c r="H82" s="12" t="s">
+      <c r="A79">
+        <v>0</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="H79" t="s">
+        <v>23</v>
+      </c>
+      <c r="I79" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>0</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="H80" t="s">
+        <v>34</v>
+      </c>
+      <c r="I80" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A83" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
+      <c r="H83" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I83" s="12" t="s">
         <v>13</v>
-      </c>
-      <c r="I82" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>1</v>
-      </c>
-      <c r="H83" t="s">
-        <v>38</v>
-      </c>
-      <c r="I83" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>0</v>
-      </c>
-      <c r="B84">
         <v>1</v>
       </c>
       <c r="H84" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="I84" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -5108,373 +5065,326 @@
         <v>0</v>
       </c>
       <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="H85" t="s">
+        <v>32</v>
+      </c>
+      <c r="I85" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86">
         <v>0</v>
       </c>
-      <c r="H85" t="s">
-        <v>39</v>
-      </c>
-      <c r="I85" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A88" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B88" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="F88" s="4"/>
-      <c r="G88" s="4"/>
-      <c r="H88" s="12" t="s">
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="H86" t="s">
+        <v>50</v>
+      </c>
+      <c r="I86" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B89" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C89" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I89" s="12" t="s">
         <v>13</v>
-      </c>
-      <c r="I88" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>1</v>
-      </c>
-      <c r="H89" t="s">
-        <v>37</v>
-      </c>
-      <c r="I89" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>0</v>
-      </c>
-      <c r="B90">
         <v>1</v>
       </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
       <c r="H90" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="I90" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
+        <v>1</v>
+      </c>
+      <c r="C91">
         <v>0</v>
       </c>
-      <c r="B91">
+      <c r="H91" t="s">
+        <v>37</v>
+      </c>
+      <c r="I91" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92">
         <v>0</v>
       </c>
-      <c r="H91" t="s">
-        <v>55</v>
-      </c>
-      <c r="I91" t="s">
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="H92" t="s">
+        <v>34</v>
+      </c>
+      <c r="I92" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B94" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C94" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="F94" s="4"/>
-      <c r="G94" s="4"/>
-      <c r="H94" s="12" t="s">
+      <c r="A93">
+        <v>0</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="H93" t="s">
+        <v>14</v>
+      </c>
+      <c r="I93" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>0</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="H94" t="s">
+        <v>50</v>
+      </c>
+      <c r="I94" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="4"/>
+      <c r="H98" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I98" s="12" t="s">
         <v>13</v>
-      </c>
-      <c r="I94" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>1</v>
-      </c>
-      <c r="C95">
-        <v>1</v>
-      </c>
-      <c r="H95" t="s">
-        <v>16</v>
-      </c>
-      <c r="I95" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>1</v>
-      </c>
-      <c r="C96">
-        <v>0</v>
-      </c>
-      <c r="H96" t="s">
-        <v>42</v>
-      </c>
-      <c r="I96" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>0</v>
-      </c>
-      <c r="B97">
-        <v>1</v>
-      </c>
-      <c r="H97" t="s">
-        <v>39</v>
-      </c>
-      <c r="I97" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>0</v>
-      </c>
-      <c r="B98">
-        <v>0</v>
-      </c>
-      <c r="C98">
-        <v>1</v>
-      </c>
-      <c r="H98" t="s">
-        <v>16</v>
-      </c>
-      <c r="I98" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
+        <v>1</v>
+      </c>
+      <c r="H99" t="s">
+        <v>56</v>
+      </c>
+      <c r="I99" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100">
         <v>0</v>
       </c>
-      <c r="B99">
+      <c r="B100">
+        <v>1</v>
+      </c>
+      <c r="H100" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I100" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101">
         <v>0</v>
       </c>
-      <c r="C99">
+      <c r="B101">
         <v>0</v>
       </c>
-      <c r="H99" t="s">
-        <v>55</v>
-      </c>
-      <c r="I99" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A103" s="4" t="s">
+      <c r="H101" t="s">
+        <v>57</v>
+      </c>
+      <c r="I101" t="s">
         <v>91</v>
       </c>
-      <c r="B103" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C103" s="4"/>
-      <c r="D103" s="4"/>
-      <c r="F103" s="4"/>
-      <c r="G103" s="4"/>
-      <c r="H103" s="12" t="s">
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B103" s="8"/>
+      <c r="C103" s="8"/>
+      <c r="D103" s="8"/>
+      <c r="E103" s="8"/>
+      <c r="F103" s="8"/>
+      <c r="G103" s="8"/>
+      <c r="H103" s="8"/>
+      <c r="I103" s="8"/>
+    </row>
+    <row r="104" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A104" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B104" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C104" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D104" s="11"/>
+      <c r="E104" s="11"/>
+      <c r="F104" s="12"/>
+      <c r="G104" s="12"/>
+      <c r="H104" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I104" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I103" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104">
+    </row>
+    <row r="105" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="13">
         <v>1</v>
       </c>
-      <c r="H104" t="s">
-        <v>61</v>
-      </c>
-      <c r="I104" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105">
+      <c r="C105" s="13"/>
+      <c r="D105" s="13"/>
+      <c r="E105" s="13"/>
+      <c r="F105" s="13"/>
+      <c r="G105" s="13"/>
+      <c r="H105" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I105" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="13">
         <v>0</v>
       </c>
-      <c r="B105">
+      <c r="B106">
         <v>1</v>
       </c>
-      <c r="H105" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I105" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106">
+      <c r="C106" s="13"/>
+      <c r="D106" s="13"/>
+      <c r="E106" s="13"/>
+      <c r="F106" s="13"/>
+      <c r="G106" s="13"/>
+      <c r="H106" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I106" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="13">
         <v>0</v>
       </c>
-      <c r="B106">
+      <c r="B107">
         <v>0</v>
       </c>
-      <c r="H106" t="s">
-        <v>62</v>
-      </c>
-      <c r="I106" t="s">
-        <v>96</v>
+      <c r="C107" s="13">
+        <v>1</v>
+      </c>
+      <c r="D107" s="13"/>
+      <c r="E107" s="13"/>
+      <c r="F107" s="13"/>
+      <c r="G107" s="13"/>
+      <c r="H107" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="I107" s="13" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="B108" s="8"/>
-      <c r="C108" s="8"/>
-      <c r="D108" s="8"/>
-      <c r="E108" s="8"/>
-      <c r="F108" s="8"/>
-      <c r="G108" s="8"/>
-      <c r="H108" s="8"/>
-      <c r="I108" s="8"/>
-    </row>
-    <row r="109" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A109" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B109" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C109" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D109" s="11"/>
-      <c r="E109" s="11"/>
-      <c r="F109" s="12"/>
-      <c r="G109" s="12"/>
-      <c r="H109" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I109" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="13">
-        <v>1</v>
-      </c>
-      <c r="C110" s="13"/>
-      <c r="D110" s="13"/>
-      <c r="E110" s="13"/>
-      <c r="F110" s="13"/>
-      <c r="G110" s="13"/>
-      <c r="H110" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="I110" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="13">
+      <c r="A108" s="13">
         <v>0</v>
       </c>
-      <c r="B111">
-        <v>1</v>
-      </c>
-      <c r="C111" s="13"/>
-      <c r="D111" s="13"/>
-      <c r="E111" s="13"/>
-      <c r="F111" s="13"/>
-      <c r="G111" s="13"/>
-      <c r="H111" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="I111" s="13" t="s">
-        <v>82</v>
+      <c r="B108">
+        <v>0</v>
+      </c>
+      <c r="C108" s="13">
+        <v>0</v>
+      </c>
+      <c r="D108" s="13"/>
+      <c r="E108" s="13"/>
+      <c r="F108" s="13"/>
+      <c r="G108" s="25"/>
+      <c r="H108" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I108" s="13" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="13">
-        <v>0</v>
-      </c>
-      <c r="B112">
-        <v>0</v>
-      </c>
-      <c r="C112" s="13">
-        <v>1</v>
-      </c>
-      <c r="D112" s="13"/>
-      <c r="E112" s="13"/>
-      <c r="F112" s="13"/>
-      <c r="G112" s="13"/>
-      <c r="H112" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="I112" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="13">
-        <v>0</v>
-      </c>
-      <c r="B113">
-        <v>0</v>
-      </c>
-      <c r="C113" s="13">
-        <v>0</v>
-      </c>
-      <c r="D113" s="13"/>
-      <c r="E113" s="13"/>
-      <c r="F113" s="13"/>
-      <c r="G113" s="25"/>
-      <c r="H113" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="I113" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H117" s="14"/>
-      <c r="I117" s="13"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H118" s="14"/>
-      <c r="I118" s="13"/>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H119" s="14"/>
-      <c r="I119" s="13"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H120" s="14"/>
-      <c r="I120" s="13"/>
+      <c r="H112" s="14"/>
+      <c r="I112" s="13"/>
+    </row>
+    <row r="113" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H113" s="14"/>
+      <c r="I113" s="13"/>
+    </row>
+    <row r="114" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H114" s="14"/>
+      <c r="I114" s="13"/>
+    </row>
+    <row r="115" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H115" s="14"/>
+      <c r="I115" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A32:K32"/>
-    <mergeCell ref="G53:G57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5495,27 +5405,27 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>